<commit_message>
Iteration v0.6 -- Spacy Lemmatization
</commit_message>
<xml_diff>
--- a/results/Results_summary.xlsx
+++ b/results/Results_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t xml:space="preserve">Iteration</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t xml:space="preserve">Undersampling training data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removed twitter pic urls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lemmatization</t>
   </si>
 </sst>
 </file>
@@ -221,8 +227,8 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -394,8 +400,8 @@
         <v>0.5</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>1</v>
+      <c r="F8" s="2" t="n">
+        <v>0.6</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="n">
@@ -459,6 +465,9 @@
       <c r="D10" s="0" t="n">
         <v>0.927020202020202</v>
       </c>
+      <c r="F10" s="0" t="n">
+        <v>0.921969696969697</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -470,6 +479,9 @@
       <c r="D11" s="0" t="n">
         <v>0.0562685093780849</v>
       </c>
+      <c r="F11" s="0" t="n">
+        <v>0.0567620927936821</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -486,6 +498,12 @@
       </c>
       <c r="E12" s="4" t="n">
         <v>0.883970739423941</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0.860810810810811</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>0.879544540363254</v>
       </c>
       <c r="I12" s="4"/>
       <c r="K12" s="4"/>
@@ -521,10 +539,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -625,6 +643,22 @@
         <v>22</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Iteration v0.7 -- Split Camel Case hashtags
</commit_message>
<xml_diff>
--- a/results/Results_summary.xlsx
+++ b/results/Results_summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t xml:space="preserve">Iteration</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t xml:space="preserve">lemmatization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">split Camel case hashtags</t>
   </si>
 </sst>
 </file>
@@ -228,7 +231,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -405,7 +408,7 @@
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="n">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="n">
@@ -468,6 +471,9 @@
       <c r="F10" s="0" t="n">
         <v>0.921969696969697</v>
       </c>
+      <c r="H10" s="0" t="n">
+        <v>0.91969696969697</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -482,6 +488,9 @@
       <c r="F11" s="0" t="n">
         <v>0.0567620927936821</v>
       </c>
+      <c r="H11" s="0" t="n">
+        <v>0.0533070088845015</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -504,6 +513,9 @@
       </c>
       <c r="G12" s="4" t="n">
         <v>0.879544540363254</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.85778175313059</v>
       </c>
       <c r="I12" s="4"/>
       <c r="K12" s="4"/>
@@ -539,10 +551,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -659,6 +671,14 @@
         <v>24</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Iteration v0.7.2 -- Additonal URL cleanup
</commit_message>
<xml_diff>
--- a/results/Results_summary.xlsx
+++ b/results/Results_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
   <si>
     <t xml:space="preserve">Iteration</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve">0.4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7.2</t>
   </si>
   <si>
     <t xml:space="preserve">Pre-processing</t>
@@ -230,8 +233,8 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -411,8 +414,8 @@
         <v>0.7</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="2" t="n">
-        <v>0.3</v>
+      <c r="J8" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="n">
@@ -474,6 +477,9 @@
       <c r="H10" s="0" t="n">
         <v>0.91969696969697</v>
       </c>
+      <c r="J10" s="0" t="n">
+        <v>0.922979797979798</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -491,6 +497,9 @@
       <c r="H11" s="0" t="n">
         <v>0.0533070088845015</v>
       </c>
+      <c r="J11" s="0" t="n">
+        <v>0.0547877591312932</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -517,8 +526,15 @@
       <c r="H12" s="0" t="n">
         <v>0.85778175313059</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="I12" s="4" t="n">
+        <v>0.870070989112258</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0.862612612612613</v>
+      </c>
+      <c r="K12" s="4" t="n">
+        <v>0.871422594308083</v>
+      </c>
       <c r="M12" s="4"/>
     </row>
   </sheetData>
@@ -553,7 +569,7 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -571,13 +587,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -585,23 +601,23 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,7 +625,7 @@
         <v>0.1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,10 +641,10 @@
         <v>0.2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,7 +652,7 @@
         <v>0.3</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -644,7 +660,7 @@
         <v>0.4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,7 +668,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -660,7 +676,7 @@
         <v>0.5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,7 +684,7 @@
         <v>0.6</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,7 +692,7 @@
         <v>0.7</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Iteration v0.7.5 -- Additonal URL cleanup
</commit_message>
<xml_diff>
--- a/results/Results_summary.xlsx
+++ b/results/Results_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="32">
   <si>
     <t xml:space="preserve">Iteration</t>
   </si>
@@ -50,6 +50,12 @@
     <t xml:space="preserve">0.7.2</t>
   </si>
   <si>
+    <t xml:space="preserve">0.7.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pre-processing</t>
   </si>
   <si>
@@ -102,6 +108,15 @@
   </si>
   <si>
     <t xml:space="preserve">split Camel case hashtags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleaned URLs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additonal URL cleanup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Url cleanup</t>
   </si>
 </sst>
 </file>
@@ -231,10 +246,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -394,163 +409,275 @@
         <v>0.885328885810059</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="n">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="n">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="n">
         <v>0.6</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="n">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="n">
         <v>0.7</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>0.89280303030303</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>0.927020202020202</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>0.921969696969697</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>0.91969696969697</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>0.922979797979798</v>
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.0227048371174729</v>
+        <v>0.89280303030303</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0.0562685093780849</v>
+        <v>0.927020202020202</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0.0567620927936821</v>
+        <v>0.921969696969697</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>0.0533070088845015</v>
+        <v>0.91969696969697</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>0.0547877591312932</v>
+        <v>0.922979797979798</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>0.919444444444444</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.0227048371174729</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.0562685093780849</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0.0567620927936821</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.0533070088845015</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0.0547877591312932</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>0.0547877591312932</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B13" s="0" t="n">
         <v>0.82345601996257</v>
       </c>
-      <c r="C12" s="4" t="n">
+      <c r="C13" s="4" t="n">
         <v>0.867071174963912</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D13" s="0" t="n">
         <v>0.868696047251249</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E13" s="4" t="n">
         <v>0.883970739423941</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F13" s="0" t="n">
         <v>0.860810810810811</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G13" s="4" t="n">
         <v>0.879544540363254</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <v>0.85778175313059</v>
       </c>
-      <c r="I12" s="4" t="n">
+      <c r="I13" s="4" t="n">
         <v>0.870070989112258</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J13" s="0" t="n">
         <v>0.862612612612613</v>
       </c>
-      <c r="K12" s="4" t="n">
+      <c r="K13" s="4" t="n">
         <v>0.871422594308083</v>
       </c>
-      <c r="M12" s="4"/>
+      <c r="L13" s="0" t="n">
+        <v>0.857206803939122</v>
+      </c>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.919444444444444</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.0547877591312932</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.857206803939122</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="M20" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -567,10 +694,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -587,13 +714,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -601,23 +728,23 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,7 +752,7 @@
         <v>0.1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,10 +768,10 @@
         <v>0.2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,7 +779,7 @@
         <v>0.3</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -660,7 +787,7 @@
         <v>0.4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,7 +795,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,7 +803,7 @@
         <v>0.5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -684,7 +811,7 @@
         <v>0.6</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,7 +819,31 @@
         <v>0.7</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Iteration v0.7.6b -- Logistic Regression
</commit_message>
<xml_diff>
--- a/results/Results_summary.xlsx
+++ b/results/Results_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
   <si>
     <t xml:space="preserve">Iteration</t>
   </si>
@@ -56,6 +56,12 @@
     <t xml:space="preserve">0.7.5</t>
   </si>
   <si>
+    <t xml:space="preserve">0.7.6b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7.6a</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pre-processing</t>
   </si>
   <si>
@@ -117,6 +123,9 @@
   </si>
   <si>
     <t xml:space="preserve">Url cleanup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logistic Regression</t>
   </si>
 </sst>
 </file>
@@ -248,8 +257,8 @@
   </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -569,12 +578,12 @@
         <v>10</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="2" t="n">
-        <v>0.5</v>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="2" t="n">
-        <v>0.6</v>
+      <c r="F16" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="n">
@@ -635,6 +644,12 @@
       <c r="B18" s="0" t="n">
         <v>0.919444444444444</v>
       </c>
+      <c r="D18" s="0" t="n">
+        <v>0.973232323232323</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0.922727272727273</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -643,6 +658,12 @@
       <c r="B19" s="0" t="n">
         <v>0.0547877591312932</v>
       </c>
+      <c r="D19" s="0" t="n">
+        <v>0.0488647581441264</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>0.0552813425468904</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -652,7 +673,13 @@
         <v>0.857206803939122</v>
       </c>
       <c r="C20" s="4"/>
+      <c r="D20" s="0" t="n">
+        <v>0.947860304968028</v>
+      </c>
       <c r="E20" s="4"/>
+      <c r="F20" s="0" t="n">
+        <v>0.862162162162162</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="I20" s="4"/>
       <c r="K20" s="4"/>
@@ -694,10 +721,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -714,13 +741,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,23 +755,23 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -752,7 +779,7 @@
         <v>0.1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -760,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,10 +795,10 @@
         <v>0.2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,7 +806,7 @@
         <v>0.3</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,7 +814,7 @@
         <v>0.4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -795,7 +822,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,7 +830,7 @@
         <v>0.5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -811,7 +838,7 @@
         <v>0.6</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,7 +846,7 @@
         <v>0.7</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,7 +854,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -835,7 +862,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,7 +870,20 @@
         <v>10</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Iteration v0.9 -- Porter Stemmer
</commit_message>
<xml_diff>
--- a/results/Results_summary.xlsx
+++ b/results/Results_summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="39">
   <si>
     <t xml:space="preserve">Iteration</t>
   </si>
@@ -62,6 +62,12 @@
     <t xml:space="preserve">0.7.6a</t>
   </si>
   <si>
+    <t xml:space="preserve">0.9a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pre-processing</t>
   </si>
   <si>
@@ -126,6 +132,12 @@
   </si>
   <si>
     <t xml:space="preserve">Logistic Regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wordninja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PorterStemmer</t>
   </si>
 </sst>
 </file>
@@ -258,7 +270,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -587,15 +599,15 @@
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="M16" s="2"/>
     </row>
@@ -650,6 +662,15 @@
       <c r="F18" s="0" t="n">
         <v>0.922727272727273</v>
       </c>
+      <c r="H18" s="0" t="n">
+        <v>0.908207070707071</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>0.913636363636364</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>0.971085858585859</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -664,6 +685,15 @@
       <c r="F19" s="0" t="n">
         <v>0.0552813425468904</v>
       </c>
+      <c r="H19" s="0" t="n">
+        <v>0.0577492596248766</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>0.052319842053307</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>0.0498519249753208</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -681,9 +711,22 @@
         <v>0.862162162162162</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="H20" s="0" t="n">
+        <v>0.84004400440044</v>
+      </c>
+      <c r="I20" s="4" t="n">
+        <v>0.876056181061124</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0.848806366047745</v>
+      </c>
       <c r="K20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="L20" s="0" t="n">
+        <v>0.943858788918853</v>
+      </c>
+      <c r="M20" s="4" t="n">
+        <v>0.855143054009646</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -721,10 +764,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="1" sqref="L16 D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -741,13 +784,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -755,23 +798,23 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,7 +822,7 @@
         <v>0.1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -795,10 +838,10 @@
         <v>0.2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -806,7 +849,7 @@
         <v>0.3</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,7 +857,7 @@
         <v>0.4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,7 +865,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,7 +873,7 @@
         <v>0.5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,7 +881,7 @@
         <v>0.6</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,7 +889,7 @@
         <v>0.7</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,7 +897,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,7 +905,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -870,7 +913,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -883,7 +926,34 @@
         <v>11</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>